<commit_message>
updated analyses and manuscript
</commit_message>
<xml_diff>
--- a/manuscript/power analyses table.xlsx
+++ b/manuscript/power analyses table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/reanalysis-of-vahey-2015/manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB66140-C738-3D4A-88C8-EE2BCDEF34F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2989251-7C5D-0A4E-AA40-FF4A44B4C0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{1835FDAE-4C49-9F48-9B57-DE64D2D554F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{1835FDAE-4C49-9F48-9B57-DE64D2D554F2}"/>
   </bookViews>
   <sheets>
     <sheet name="power analyses" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Point estimate</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Reported as Field &amp; Gillett's (2010) SPSS script, but code not shared upon request</t>
-  </si>
-  <si>
-    <t>Viechtbauer's R script using the metafor R package</t>
   </si>
   <si>
     <t>Lower</t>
@@ -122,62 +119,62 @@
     <t>required_n_new</t>
   </si>
   <si>
-    <t>Field &amp; Gillett's (2010) "h_s syntax.sps" SPSS script</t>
-  </si>
-  <si>
-    <t>Field &amp; Gillett's (2010) "Meta_Basic_r.sps" SPSS script</t>
-  </si>
-  <si>
-    <t>NaN</t>
-  </si>
-  <si>
     <t>Modifications</t>
   </si>
   <si>
-    <t>CIs calculated using SE</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Field &amp; Gillett's (2010) "Meta_Basic_r.sps" SPSS script rewritten in R</t>
-  </si>
-  <si>
     <t>All reliabilities set to 0</t>
   </si>
   <si>
-    <t>Fisher's r-to-z transformations prior to analysis and z-to-r back transformations prior to reporting</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
-    <t>Hunter &amp; Schmidt method (implementation 1)</t>
-  </si>
-  <si>
-    <t>Hunter &amp; Schmidt method (implementation 2)</t>
-  </si>
-  <si>
-    <t>Hunter &amp; Schmidt method (implementation 3)</t>
-  </si>
-  <si>
-    <t>Mix of Hunter &amp; Schmidt and Hedges &amp; colleages' methods</t>
-  </si>
-  <si>
-    <t>CIs calculated using SE, inapprorpriate Overton transformations removed</t>
-  </si>
-  <si>
-    <t>Hunter &amp; Schmidt method (implementation 1 corrected)</t>
-  </si>
-  <si>
-    <t>Unknown</t>
+    <t>Correction to set variance in population correlations to zero if it is negative, as in "h_s_ syntax.sps"</t>
+  </si>
+  <si>
+    <t>Correction to set variance in population correlations to zero if it is negative, as in "h_s_ syntax.sps", inapprorpriate Overton transformations removed</t>
+  </si>
+  <si>
+    <t>Not calculated</t>
+  </si>
+  <si>
+    <t>Verification attempt 1: Hunter &amp; Schmidt method (implementation 1)</t>
+  </si>
+  <si>
+    <t>Unkown</t>
+  </si>
+  <si>
+    <t>Verification attempt 2: Hunter &amp; Schmidt method (implementation 2)</t>
+  </si>
+  <si>
+    <t>Verification attempt 3: Hunter &amp; Schmidt method (implementation 2)</t>
+  </si>
+  <si>
+    <t>Verification attempt 4: Hunter &amp; Schmidt method (implementation 3)</t>
+  </si>
+  <si>
+    <t>Verification attempt 5: Mix of Hunter &amp; Schmidt and Hedges' methods</t>
+  </si>
+  <si>
+    <t>Field &amp; Gillett's (2010) Basic meta-analysis</t>
+  </si>
+  <si>
+    <t>Viechtbauer's Hunter &amp; Schmidt style meta-analysis</t>
+  </si>
+  <si>
+    <t>Field &amp; Gillett's (2010) Hunter &amp; Schmidt style meta-analysis</t>
+  </si>
+  <si>
+    <t>Credibility intervals were implemented using Field &amp; Gillett's (2010) equations</t>
+  </si>
+  <si>
+    <t>Credibility intervals were implemented using Field &amp; Gillett's (2010) equations, Fisher's r-to-z transformations prior to analysis and z-to-r back transformations prior to reporting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,8 +189,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,12 +213,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,21 +261,21 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,41 +621,41 @@
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>0.45</v>
       </c>
       <c r="E3">
@@ -666,24 +664,24 @@
       <c r="F3">
         <v>29</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <v>0.18</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="7">
         <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>0.4</v>
       </c>
       <c r="E4">
@@ -692,24 +690,24 @@
       <c r="F4">
         <v>37</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>0.1</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="7">
         <v>617</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>0.45</v>
       </c>
       <c r="E5">
@@ -718,47 +716,47 @@
       <c r="F5">
         <v>36</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>0.18</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="7">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>0.4</v>
       </c>
       <c r="F6">
         <v>46</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>0.1</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="7">
         <v>782</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>1.01</v>
       </c>
       <c r="E7">
@@ -767,50 +765,50 @@
       <c r="F7">
         <v>26</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="10">
         <v>0.37</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="7">
         <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>0.87</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>36</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <v>34</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="10">
         <v>0.2</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="7">
         <v>614</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>1.01</v>
       </c>
       <c r="E9">
@@ -819,24 +817,24 @@
       <c r="F9">
         <v>8</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="10">
         <v>0.37</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="7">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="7">
         <v>0.87</v>
       </c>
       <c r="E10">
@@ -845,16 +843,16 @@
       <c r="F10">
         <v>10</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="10">
         <v>0.2</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="7">
         <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="3" customFormat="1" ht="238" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -867,15 +865,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4930379-F378-9D4C-A870-F0AD0F86B1AA}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="43" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="43" style="2" customWidth="1"/>
+    <col min="5" max="6" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -886,30 +886,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
       <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -920,7 +920,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4">
         <v>0.45</v>
@@ -939,118 +939,118 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.47</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.74</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0.47</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.46</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.46</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.47</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0.47</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.47</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.54</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.47</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.46</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0.47</v>
-      </c>
-      <c r="H4" s="8">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.46</v>
-      </c>
-      <c r="E5" s="13">
-        <v>0.19</v>
-      </c>
-      <c r="F5" s="13">
-        <v>0.73</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.47</v>
-      </c>
-      <c r="E6" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="F6" s="13">
-        <v>0.74</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0.31</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.47</v>
-      </c>
-      <c r="E7" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="F7" s="13">
-        <v>0.74</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0.47</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D8" s="5">
         <v>0.47</v>
@@ -1061,38 +1061,17 @@
       <c r="F8" s="6">
         <v>0.54</v>
       </c>
-      <c r="G8" s="7">
-        <v>0.47</v>
-      </c>
-      <c r="H8" s="8">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.47</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0.54</v>
-      </c>
-      <c r="G9" s="7">
-        <v>0.47</v>
-      </c>
-      <c r="H9" s="8">
-        <v>0.47</v>
-      </c>
+      <c r="G8" s="13">
+        <v>0.47</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -1114,11 +1093,6 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>